<commit_message>
docs (updated): Se añadieron algunos requerimientos.
</commit_message>
<xml_diff>
--- a/Documentación/Planilla_de_Requerimientos.xlsx
+++ b/Documentación/Planilla_de_Requerimientos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitsf\Desktop\Capstone\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3860ACCA-EB61-4A64-B4EB-ED4BC312C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF895085-57FC-499D-B529-1D26943CCE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Ejemplo" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Requerimiento Inicial'!$A$1:$F$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Requerimiento Inicial'!$A$1:$F$41</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="134">
   <si>
     <t>[R-N°]</t>
   </si>
@@ -258,18 +258,12 @@
     <t>Los usuarios y distribuidores podrán iniciar sesión utilizando sus credenciales registradas.</t>
   </si>
   <si>
-    <t>Usuario, Proveedor y Administrador</t>
-  </si>
-  <si>
     <t>Perfiles de Usuario</t>
   </si>
   <si>
     <t>Los usuarios tendrán perfiles que mostrarán información básica, historial de pedidos, métodos de pago preferidos, y direcciones de entrega guardadas.</t>
   </si>
   <si>
-    <t>Usuario y Proveedor</t>
-  </si>
-  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -420,20 +414,32 @@
     <t>Compartir Ubicación en Tiempo Real</t>
   </si>
   <si>
-    <t>Usuario, Proveedor</t>
-  </si>
-  <si>
     <t>Permitir a los usuarios compartir su ubicación en tiempo real con el distribuidor para facilitar la entrega.</t>
   </si>
   <si>
     <t>Requisitos técnicos del sistema</t>
+  </si>
+  <si>
+    <t>Mensajería Interna</t>
+  </si>
+  <si>
+    <t>Usuario, Distribuidor</t>
+  </si>
+  <si>
+    <t>Usuario, Distribuidor y Administrador</t>
+  </si>
+  <si>
+    <t>Usuario y Distribuidor</t>
+  </si>
+  <si>
+    <t>Chat en tiempo real entre el usuario y el distribuidor.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -481,6 +487,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -591,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -642,6 +653,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -925,7 +937,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>73</v>
@@ -943,7 +955,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>74</v>
@@ -961,7 +973,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>13</v>
@@ -973,16 +985,16 @@
         <v>14</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="15"/>
     </row>
@@ -997,10 +1009,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F6" s="15"/>
     </row>
@@ -1009,16 +1021,16 @@
         <v>17</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F7" s="15"/>
     </row>
@@ -1033,7 +1045,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>20</v>
@@ -1045,16 +1057,16 @@
         <v>21</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="15"/>
     </row>
@@ -1063,16 +1075,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F10" s="15"/>
     </row>
@@ -1081,16 +1093,16 @@
         <v>23</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F11" s="15"/>
     </row>
@@ -1099,16 +1111,16 @@
         <v>24</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F12" s="15"/>
     </row>
@@ -1117,16 +1129,16 @@
         <v>25</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" s="15"/>
     </row>
@@ -1135,16 +1147,16 @@
         <v>26</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F14" s="15"/>
     </row>
@@ -1153,16 +1165,16 @@
         <v>27</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F15" s="15"/>
     </row>
@@ -1170,17 +1182,17 @@
       <c r="A16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>128</v>
+      <c r="B16" s="20" t="s">
+        <v>126</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>129</v>
+      <c r="D16" s="20" t="s">
+        <v>130</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F16" s="15"/>
     </row>
@@ -1188,17 +1200,17 @@
       <c r="A17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>126</v>
+      <c r="B17" s="20" t="s">
+        <v>129</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>79</v>
+      <c r="D17" s="20" t="s">
+        <v>130</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F17" s="15"/>
     </row>
@@ -1206,17 +1218,17 @@
       <c r="A18" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>98</v>
+      <c r="B18" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="F18" s="15"/>
     </row>
@@ -1225,16 +1237,16 @@
         <v>31</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>131</v>
+        <v>8</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>98</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F19" s="15"/>
     </row>
@@ -1243,16 +1255,16 @@
         <v>33</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>131</v>
+        <v>100</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F20" s="15"/>
     </row>
@@ -1261,16 +1273,16 @@
         <v>35</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="C21" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>106</v>
       </c>
       <c r="F21" s="15"/>
     </row>
@@ -1279,16 +1291,16 @@
         <v>36</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F22" s="15"/>
     </row>
@@ -1297,16 +1309,16 @@
         <v>37</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F23" s="15"/>
     </row>
@@ -1315,16 +1327,16 @@
         <v>38</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F24" s="15"/>
     </row>
@@ -1333,16 +1345,16 @@
         <v>39</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>131</v>
+        <v>100</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>128</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F25" s="15"/>
     </row>
@@ -1351,16 +1363,16 @@
         <v>40</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F26" s="15"/>
     </row>
@@ -1369,16 +1381,16 @@
         <v>41</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F27" s="15"/>
     </row>
@@ -1387,16 +1399,16 @@
         <v>42</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F28" s="15"/>
     </row>
@@ -1405,78 +1417,86 @@
         <v>43</v>
       </c>
       <c r="B29" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="17" t="s">
+      <c r="C31" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="16" t="s">
+      <c r="F31" s="15"/>
+    </row>
+    <row r="32" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="15"/>
-    </row>
-    <row r="31" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1486,7 +1506,7 @@
     </row>
     <row r="35" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1496,7 +1516,7 @@
     </row>
     <row r="36" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1506,7 +1526,7 @@
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1516,7 +1536,7 @@
     </row>
     <row r="38" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1526,7 +1546,7 @@
     </row>
     <row r="39" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1536,7 +1556,7 @@
     </row>
     <row r="40" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1545,6 +1565,9 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -1558,7 +1581,13 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
     <row r="44" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="46" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2516,8 +2545,10 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <autoFilter ref="A1:F40" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F41" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
docs (updated): Se agrega un requerimiento más a los existentes
</commit_message>
<xml_diff>
--- a/Documentación/Planilla_de_Requerimientos.xlsx
+++ b/Documentación/Planilla_de_Requerimientos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitsf\Desktop\Capstone\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF895085-57FC-499D-B529-1D26943CCE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB88004-C4D2-456E-930A-DBA1CC3513C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -872,7 +872,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>